<commit_message>
Minor updates to kicad files
</commit_message>
<xml_diff>
--- a/Fabrication/MiniDelay v1.0 - BOM.xlsx
+++ b/Fabrication/MiniDelay v1.0 - BOM.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="158">
   <si>
     <t xml:space="preserve">Part No.</t>
   </si>
@@ -83,409 +83,418 @@
     <t xml:space="preserve">22uF</t>
   </si>
   <si>
+    <t xml:space="preserve">Murata Electronics </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRM21BR61E226ME44L </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multilayer Ceramic Capacitors MLCC - SMD/SMT 22UF 25V 20% 0805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surface mount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C49678</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C10 C12 C15 C19 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.2nF</t>
+  </si>
+  <si>
     <t xml:space="preserve">YAGEO</t>
   </si>
   <si>
+    <t xml:space="preserve">CC0603JRNPO9BN222</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multilayer Ceramic Capacitors MLCC - SMD/SMT 50V 2200pF C0G 0603 5% </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C107043</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C14 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">330nF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC0603KRX7R8BB334</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multilayer Ceramic Capacitors MLCC - SMD/SMT 25V 0.33uF X7R 0603 10% </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C107070</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C16 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">15nF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AC0603KRX7R0BB153</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multilayer Ceramic Capacitors MLCC - SMD/SMT 100 V 0.015 uF X7R 0603 10% AEC-Q200 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C2210963</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C20 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.7nF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC0603JRX7R9BB472</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multilayer Ceramic Capacitors MLCC - SMD/SMT 50V 4700pF X7R 0603 5% </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C115060</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C21 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10nF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC0603JRX7R9BB103</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multilayer Ceramic Capacitors MLCC - SMD/SMT 50V 0.01uF X7R 0603 5%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C115056</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C22 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">68pF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC0603GRNPO9BN680</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multilayer Ceramic Capacitors MLCC - SMD/SMT 50 V 68 pF C0G 0603 2%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C519457</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C3 C4 C8 C9 C11 C13 C17 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">100nF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC0603JRX7R9BB104</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multilayer Ceramic Capacitors MLCC - SMD/SMT 50 V 0.1uF X7R 0603 5% </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C91183</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">220nF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Murata Electronics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GCM188R71H224KA64D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multilayer Ceramic Capacitors MLCC - SMD/SMT .22UF 50V 10% 0603</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C97857</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">47pF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC0603JRNPO9BN470</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multilayer Ceramic Capacitors MLCC - SMD/SMT 50 V 47 pF C0G 0603 5% </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C105622</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C7 C18 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1uF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taiyo Yuden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UMK107AB7105KA-T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multilayer Ceramic Capacitors MLCC - SMD/SMT 0603 50VDC 1uF 10% X7R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C105174</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3mm_LED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EKINGLUX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EL304RD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.0mm Round Through Hole LED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C2856645</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IDC_2x05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XKB Connectivity </t>
+  </si>
+  <si>
+    <t xml:space="preserve">X9555WV-2X05-6TV01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IDC Connector 2x05 2.54mm Pitch Straight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C706914</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEVEL1 REPEATS1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">B10k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alpha (Taiwan)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RD901F-40-15R1-B10K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10K OHM Linear Taper Potentiometer Round Shaft PCB 9mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RD901F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R1 R16 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0603FR-071ML</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thick Film Resistors - SMD 1 MOhms 100mW 0603 1% </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C105578</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R18 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">68k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0603FR-0768KL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thick Film Resistors - SMD 68 kOhms 100mW 0603 1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C114633</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R2 R4 R8 R10 R11 R12 R13 R14 R15 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AC0603FR-0710KL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thick Film Resistors - SMD 10 kOhms 100mW 0603 1% AEC-Q200 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C116677</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R3 R6 R17 R20 R21 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">100k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0603FR-07100KL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thick Film Resistors - SMD 100 kOhms 100mW 0603 1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C14675</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.7k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0603FR-072K7L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thick Film Resistors - SMD 2.7 kOhms 100mW 0603 1% </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C114612</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R7 R19 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">20k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0603FR-0720KL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thick Film Resistors - SMD 20 kOhms 100mW 0603 1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C105575</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R9 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0603FR-071KL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thick Film Resistors - SMD 1 kOhms 100mW 0603 1% </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C22548</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TIME1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">B100k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RD901F-40-15R1-B100K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100K OHM Linear Taper Potentiometer Round Shaft PCB 9mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TL074</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STMicroelectronics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TL074IDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operational Amplifiers - Op Amps Quad Low Noise JFET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C107644</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOIC-14_150mil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PT2399</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PTC(Princeton Tech)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PT2399-SN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PT2399-SN </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOP-16_150mil Audio Interface ICs ROHS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C126407</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOP-16_150mil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L7805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L7805CDT-TR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">62dB@(120Hz) 1.5A 2V@(1A) Fixed 5V~5V Positive 1 35V TO-252-3 Linear Voltage Regulators (LDO) ROHS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C310413</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TO-252-3</t>
+  </si>
+  <si>
     <t xml:space="preserve">CC0805KRX7R9BB104</t>
   </si>
   <si>
     <t xml:space="preserve">Multilayer Ceramic Capacitors MLCC - SMD/SMT 50 V 0.1uF X7R 0805 10% </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surface mount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C49678</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C10 C12 C15 C19 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.2nF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CC0603JRNPO9BN222</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multilayer Ceramic Capacitors MLCC - SMD/SMT 50V 2200pF C0G 0603 5% </t>
-  </si>
-  <si>
-    <t xml:space="preserve">C107043</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C14 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">330nF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CC0603KRX7R8BB334</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multilayer Ceramic Capacitors MLCC - SMD/SMT 25V 0.33uF X7R 0603 10% </t>
-  </si>
-  <si>
-    <t xml:space="preserve">C107070</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C16 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">15nF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AC0603KRX7R0BB153</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multilayer Ceramic Capacitors MLCC - SMD/SMT 100 V 0.015 uF X7R 0603 10% AEC-Q200 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">C2210963</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C20 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.7nF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CC0603JRX7R9BB472</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multilayer Ceramic Capacitors MLCC - SMD/SMT 50V 4700pF X7R 0603 5% </t>
-  </si>
-  <si>
-    <t xml:space="preserve">C115060</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C21 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">10nF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CC0603JRX7R9BB103</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multilayer Ceramic Capacitors MLCC - SMD/SMT 50V 0.01uF X7R 0603 5%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C115056</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C22 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">68pF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CC0603GRNPO9BN680</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multilayer Ceramic Capacitors MLCC - SMD/SMT 50 V 68 pF C0G 0603 2%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C519457</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C3 C4 C8 C9 C11 C13 C17 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">100nF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CC0603JRX7R9BB104</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multilayer Ceramic Capacitors MLCC - SMD/SMT 50 V 0.1uF X7R 0603 5% </t>
-  </si>
-  <si>
-    <t xml:space="preserve">C91183</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C5 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">220nF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Murata Electronics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GCM188R71H224KA64D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multilayer Ceramic Capacitors MLCC - SMD/SMT .22UF 50V 10% 0603</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C97857</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C6 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">47pF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CC0603JRNPO9BN470</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multilayer Ceramic Capacitors MLCC - SMD/SMT 50 V 47 pF C0G 0603 5% </t>
-  </si>
-  <si>
-    <t xml:space="preserve">C105622</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C7 C18 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1uF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Taiyo Yuden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UMK107AB7105KA-T</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multilayer Ceramic Capacitors MLCC - SMD/SMT 0603 50VDC 1uF 10% X7R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C105174</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3mm_LED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EKINGLUX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EL304RD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.0mm Round Through Hole LED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C2856645</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IDC_2x05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XKB Connectivity </t>
-  </si>
-  <si>
-    <t xml:space="preserve">X9555WV-2X05-6TV01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IDC Connector 2x05 2.54mm Pitch Straight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C706914</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LEVEL1 REPEATS1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">B10k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alpha (Taiwan)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RD901F-40-15R1-B10K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10K OHM Linear Taper Potentiometer Round Shaft PCB 9mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RD901F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R1 R16 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0603FR-071ML</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thick Film Resistors - SMD 1 MOhms 100mW 0603 1% </t>
-  </si>
-  <si>
-    <t xml:space="preserve">C105578</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R18 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">68k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0603FR-0768KL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thick Film Resistors - SMD 68 kOhms 100mW 0603 1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C114633</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R2 R4 R8 R10 R11 R12 R13 R14 R15 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">10k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AC0603FR-0710KL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thick Film Resistors - SMD 10 kOhms 100mW 0603 1% AEC-Q200 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">C116677</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R3 R6 R17 R20 R21 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">100k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0603FR-07100KL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thick Film Resistors - SMD 100 kOhms 100mW 0603 1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C14675</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R5 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.7k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0603FR-072K7L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thick Film Resistors - SMD 2.7 kOhms 100mW 0603 1% </t>
-  </si>
-  <si>
-    <t xml:space="preserve">C114612</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R7 R19 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">20k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0603FR-0720KL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thick Film Resistors - SMD 20 kOhms 100mW 0603 1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C105575</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R9 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0603FR-071KL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thick Film Resistors - SMD 1 kOhms 100mW 0603 1% </t>
-  </si>
-  <si>
-    <t xml:space="preserve">C22548</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TIME1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">B100k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RD901F-40-15R1-B100K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100K OHM Linear Taper Potentiometer Round Shaft PCB 9mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TL074</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STMicroelectronics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TL074IDT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Operational Amplifiers - Op Amps Quad Low Noise JFET</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C107644</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOIC-14_150mil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">PT2399</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PTC(Princeton Tech)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PT2399-SN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PT2399-SN </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOP-16_150mil Audio Interface ICs ROHS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C126407</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOP-16_150mil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">L7805</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L7805CDT-TR </t>
-  </si>
-  <si>
-    <t xml:space="preserve">62dB@(120Hz) 1.5A 2V@(1A) Fixed 5V~5V Positive 1 35V TO-252-3 Linear Voltage Regulators (LDO) ROHS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C310413</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TO-252-3</t>
   </si>
 </sst>
 </file>
@@ -688,15 +697,15 @@
   </sheetPr>
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.36"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="28.4"/>
@@ -826,22 +835,22 @@
         <v>26</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K4" s="5" t="n">
         <v>603</v>
@@ -852,31 +861,31 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C5" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I5" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K5" s="5" t="n">
         <v>603</v>
@@ -887,31 +896,31 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C6" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K6" s="5" t="n">
         <v>603</v>
@@ -922,31 +931,31 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C7" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K7" s="5" t="n">
         <v>603</v>
@@ -957,31 +966,31 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C8" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K8" s="5" t="n">
         <v>603</v>
@@ -992,31 +1001,31 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C9" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I9" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="K9" s="5" t="n">
         <v>603</v>
@@ -1027,31 +1036,31 @@
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C10" s="5" t="n">
         <v>7</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I10" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="K10" s="5" t="n">
         <v>603</v>
@@ -1062,31 +1071,31 @@
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C11" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K11" s="5" t="n">
         <v>603</v>
@@ -1097,31 +1106,31 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C12" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I12" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K12" s="5" t="n">
         <v>603</v>
@@ -1132,31 +1141,31 @@
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C13" s="5" t="n">
         <v>2</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I13" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K13" s="5" t="n">
         <v>603</v>
@@ -1167,31 +1176,31 @@
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C14" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I14" s="6" t="s">
         <v>16</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K14" s="5" t="s">
         <v>17</v>
@@ -1202,31 +1211,31 @@
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C15" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I15" s="6" t="s">
         <v>16</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K15" s="5" t="s">
         <v>17</v>
@@ -1237,25 +1246,25 @@
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C16" s="5" t="n">
         <v>2</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I16" s="6" t="s">
         <v>16</v>
@@ -1264,7 +1273,7 @@
         <v>17</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1272,31 +1281,31 @@
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C17" s="5" t="n">
         <v>2</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="I17" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K17" s="5" t="n">
         <v>603</v>
@@ -1307,31 +1316,31 @@
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C18" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I18" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="K18" s="5" t="n">
         <v>603</v>
@@ -1342,31 +1351,31 @@
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C19" s="5" t="n">
         <v>9</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I19" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K19" s="5" t="n">
         <v>603</v>
@@ -1377,31 +1386,31 @@
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C20" s="5" t="n">
         <v>5</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="I20" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="K20" s="5" t="n">
         <v>603</v>
@@ -1412,31 +1421,31 @@
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C21" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I21" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="K21" s="5" t="n">
         <v>603</v>
@@ -1447,31 +1456,31 @@
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C22" s="5" t="n">
         <v>2</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="I22" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="K22" s="5" t="n">
         <v>603</v>
@@ -1482,31 +1491,31 @@
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C23" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I23" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="K23" s="5" t="n">
         <v>603</v>
@@ -1517,25 +1526,25 @@
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C24" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="I24" s="6" t="s">
         <v>16</v>
@@ -1544,7 +1553,7 @@
         <v>17</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1552,34 +1561,34 @@
         <v>24</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C25" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="I25" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1587,34 +1596,34 @@
         <v>25</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C26" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I26" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1622,34 +1631,34 @@
         <v>26</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C27" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="I27" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1680,11 +1689,11 @@
       <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.36"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="28.4"/>
@@ -1744,16 +1753,16 @@
         <v>19</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>21</v>
+        <v>156</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>21</v>
+        <v>156</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>22</v>
+        <v>157</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>23</v>
@@ -1779,22 +1788,22 @@
         <v>26</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K3" s="5" t="n">
         <v>603</v>
@@ -1805,31 +1814,31 @@
         <v>4</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C4" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K4" s="5" t="n">
         <v>603</v>
@@ -1840,31 +1849,31 @@
         <v>5</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C5" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I5" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K5" s="5" t="n">
         <v>603</v>
@@ -1875,31 +1884,31 @@
         <v>6</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C6" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K6" s="5" t="n">
         <v>603</v>
@@ -1910,31 +1919,31 @@
         <v>7</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C7" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K7" s="5" t="n">
         <v>603</v>
@@ -1945,31 +1954,31 @@
         <v>8</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C8" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="K8" s="5" t="n">
         <v>603</v>
@@ -1980,31 +1989,31 @@
         <v>9</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C9" s="5" t="n">
         <v>7</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I9" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="K9" s="5" t="n">
         <v>603</v>
@@ -2015,31 +2024,31 @@
         <v>10</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C10" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I10" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K10" s="5" t="n">
         <v>603</v>
@@ -2050,31 +2059,31 @@
         <v>11</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C11" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K11" s="5" t="n">
         <v>603</v>
@@ -2085,31 +2094,31 @@
         <v>12</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C12" s="5" t="n">
         <v>2</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I12" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K12" s="5" t="n">
         <v>603</v>
@@ -2120,31 +2129,31 @@
         <v>16</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C13" s="5" t="n">
         <v>2</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="I13" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K13" s="5" t="n">
         <v>603</v>
@@ -2155,31 +2164,31 @@
         <v>17</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C14" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I14" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="K14" s="5" t="n">
         <v>603</v>
@@ -2190,31 +2199,31 @@
         <v>18</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C15" s="5" t="n">
         <v>9</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I15" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K15" s="5" t="n">
         <v>603</v>
@@ -2225,31 +2234,31 @@
         <v>19</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C16" s="5" t="n">
         <v>5</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="I16" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="K16" s="5" t="n">
         <v>603</v>
@@ -2260,31 +2269,31 @@
         <v>20</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C17" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I17" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="K17" s="5" t="n">
         <v>603</v>
@@ -2295,31 +2304,31 @@
         <v>21</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C18" s="5" t="n">
         <v>2</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="I18" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="K18" s="5" t="n">
         <v>603</v>
@@ -2330,31 +2339,31 @@
         <v>22</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C19" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I19" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="K19" s="5" t="n">
         <v>603</v>
@@ -2365,34 +2374,34 @@
         <v>24</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C20" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="I20" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2400,34 +2409,34 @@
         <v>25</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C21" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I21" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2435,34 +2444,34 @@
         <v>26</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C22" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="I22" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>